<commit_message>
Primitive interface for MirrorMe
I now want to edit names and values, and see their consequences in templates and instances...
</commit_message>
<xml_diff>
--- a/MirrorMe/MirrorMe - Example.xlsx
+++ b/MirrorMe/MirrorMe - Example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="7440"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7440"/>
   </bookViews>
   <sheets>
     <sheet name="MirroMe Voorbeeldredenering" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
   <si>
     <t>TText</t>
   </si>
@@ -67,54 +67,9 @@
     <t>Scope</t>
   </si>
   <si>
-    <t>TText_08</t>
-  </si>
-  <si>
     <t>Zaak_X123</t>
   </si>
   <si>
-    <t>Op grond van [6.] en [7.] kan de DG-Bel geen voorzitter zijn van de ondernemingsraad.</t>
-  </si>
-  <si>
-    <t>6.</t>
-  </si>
-  <si>
-    <t>7.</t>
-  </si>
-  <si>
-    <t>4.</t>
-  </si>
-  <si>
-    <t>5.</t>
-  </si>
-  <si>
-    <t>1.</t>
-  </si>
-  <si>
-    <t>2.</t>
-  </si>
-  <si>
-    <t>3.</t>
-  </si>
-  <si>
-    <t>8.</t>
-  </si>
-  <si>
-    <t>De ondernemingsraad kiest uit zijn midden een voorzitter. [art. 7 WOR]</t>
-  </si>
-  <si>
-    <t>Op grond van [4.] en [5.] is de DG-Bel niet verkiesbaar tot lid van de ondernemingsraad.</t>
-  </si>
-  <si>
-    <t>Verkiesbaar tot lid van de ondernemingsraad zijn de personen die gedurende ten minste een jaar in de onderneming werkzaam zijn geweest. [art. 6 lid 3 WOR]</t>
-  </si>
-  <si>
-    <t>Omdat de DG-Bel bestuurder is (ogv [2.]) wordt hij voor de WOR geacht niet te behoren tot de in de Belastingdienst werkzame personen (ogv [3.]).</t>
-  </si>
-  <si>
-    <t>Voor de toepassing van het bij of krachtens de WOR bepaalde wordt de bestuurder geacht niet te behoren tot de in de onderneming werkzame personen. [art. 1 lid 4 WOR].</t>
-  </si>
-  <si>
     <t>art. 1 lid 1 sub c WOR</t>
   </si>
   <si>
@@ -130,52 +85,49 @@
     <t>art. 7 WOR</t>
   </si>
   <si>
-    <t>WOR</t>
-  </si>
-  <si>
-    <t>Wet op de Ondernemingsraden (http://wetten.overheid.nl/BWBR0002747)</t>
-  </si>
-  <si>
-    <t>onderneming: elk in de maatschappij als zelfstandige eenheid optredend organisatorisch verband waarin krachtens arbeidsovereenkomst of krachtens publiekrechtelijke aanstelling arbeid wordt verricht;</t>
-  </si>
-  <si>
-    <t>bestuurder: hij die alleen dan wel te zamen met anderen in een onderneming rechtstreeks de hoogste zeggenschap uitoefent bij de leiding van de arbeid;</t>
-  </si>
-  <si>
-    <t>Voor de toepassing van het bij of krachtens deze wet bepaalde worden de bestuurder of de bestuurders van een onderneming geacht niet te behoren tot de in de onderneming werkzame personen.</t>
-  </si>
-  <si>
-    <t>Verkiesbaar tot lid van de ondernemingsraad zijn de personen die gedurende ten minste een jaar in de onderneming werkzaam zijn geweest.</t>
-  </si>
-  <si>
-    <t>De ondernemingsraad kiest uit zijn midden een voorzitter en een of meer plaatsvervangende voorzitters. De voorzitter, of bij diens verhindering een plaatsvervangende voorzitter, vertegenwoordigt de ondernemingsraad in rechte.</t>
-  </si>
-  <si>
-    <t>TText_09</t>
-  </si>
-  <si>
-    <t>TText_10</t>
-  </si>
-  <si>
-    <t>TText_11</t>
-  </si>
-  <si>
-    <t>TText_12</t>
-  </si>
-  <si>
-    <t>TText_13</t>
-  </si>
-  <si>
-    <t>TText_14</t>
-  </si>
-  <si>
-    <t>klopt</t>
-  </si>
-  <si>
-    <t>De Belastingdienst is een onderneming in de zin van de Wet op de ondernemingsraden  [art. 1 lid 1 sub c WOR], omdat het een in de maatschappij als zelfstandige eenheid optredend organisatorisch verband is, waarin krachtens arbeidsovereenkomst of krachtens publiekrechtelijke aanstelling arbeid wordt verricht.</t>
-  </si>
-  <si>
-    <t>De DG-Bel is bestuurder in de zin van de Wet op de ondernemingsraden [art. 1 lid 1 sub e WOR], omdat hij in de Belastingdienst de hoogste zeggenschap uitoefent bij de leiding van de arbeid.</t>
+    <t>onderneming</t>
+  </si>
+  <si>
+    <t>Belastingdienst</t>
+  </si>
+  <si>
+    <t>bestuurder</t>
+  </si>
+  <si>
+    <t>DG-Bel</t>
+  </si>
+  <si>
+    <t>De Belastingdienst is een onderneming in de zin van de Wet op de ondernemingsraden, omdat het een in de maatschappij als zelfstandige eenheid optredend organisatorisch verband is, waarin krachtens arbeidsovereenkomst of krachtens publiekrechtelijke aanstelling arbeid wordt verricht.</t>
+  </si>
+  <si>
+    <t>Voor de toepassing van het bij of krachtens de WOR bepaalde wordt de [bestuurder] geacht niet te behoren tot de in de [onderneming] werkzame personen.</t>
+  </si>
+  <si>
+    <t>Verkiesbaar tot lid van de ondernemingsraad zijn de personen die gedurende ten minste een jaar in de [onderneming] werkzaam zijn geweest.</t>
+  </si>
+  <si>
+    <t>De ondernemingsraad kiest uit zijn midden een voorzitter.</t>
+  </si>
+  <si>
+    <t>De [bestuurder] is niet verkiesbaar tot lid van de ondernemingsraad.</t>
+  </si>
+  <si>
+    <t>TText_03, TText_04</t>
+  </si>
+  <si>
+    <t>TText_05, TText_06</t>
+  </si>
+  <si>
+    <t>De DG-Bel is bestuurder in de zin van de Wet op de ondernemingsraden, omdat hij in de [onderneming] de hoogste zeggenschap uitoefent bij de leiding van de arbeid.</t>
+  </si>
+  <si>
+    <t>legalGround</t>
+  </si>
+  <si>
+    <t>LegalGround</t>
+  </si>
+  <si>
+    <t>De [bestuurder] kan geen voorzitter zijn van de ondernemingsraad van de [onderneming].</t>
   </si>
 </sst>
 </file>
@@ -224,7 +176,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -242,16 +194,21 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Neutraal" xfId="1" builtinId="28"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -264,9 +221,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Kantoor">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -304,7 +261,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Kantoor">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -376,7 +333,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Kantoor">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -550,24 +507,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="9.77734375" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.88671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="78.88671875" style="8" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" style="3" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="3"/>
+    <col min="1" max="1" width="10.7109375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="79.42578125" style="9" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="8.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -583,8 +540,11 @@
       <c r="E1" s="6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F1" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -600,221 +560,119 @@
       <c r="E2" s="6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="E6" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="4" t="s">
+      <c r="E9" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Distinguish between binding and template by specialization.
Both are TTexts. The distinction is necessary, because I want to insert and delete TTexts.
I also want to have different areas in the interface for bindings and templates.
In order to get editable expressions in the interfaces, it is necessary to make the distinction.
</commit_message>
<xml_diff>
--- a/MirrorMe/MirrorMe - Example.xlsx
+++ b/MirrorMe/MirrorMe - Example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7440"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7380"/>
   </bookViews>
   <sheets>
     <sheet name="MirroMe Voorbeeldredenering" sheetId="1" r:id="rId1"/>
@@ -14,10 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
-  <si>
-    <t>TText</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="40">
   <si>
     <t>ttScope</t>
   </si>
@@ -28,18 +25,12 @@
     <t>ttTemplate</t>
   </si>
   <si>
-    <t>[TTexts]</t>
-  </si>
-  <si>
     <t>TTValue</t>
   </si>
   <si>
     <t>TTPhrase</t>
   </si>
   <si>
-    <t>TTName</t>
-  </si>
-  <si>
     <t>ttName</t>
   </si>
   <si>
@@ -109,9 +100,6 @@
     <t>De ondernemingsraad kiest uit zijn midden een voorzitter.</t>
   </si>
   <si>
-    <t>De [bestuurder] is niet verkiesbaar tot lid van de ondernemingsraad.</t>
-  </si>
-  <si>
     <t>TText_03, TText_04</t>
   </si>
   <si>
@@ -128,6 +116,24 @@
   </si>
   <si>
     <t>De [bestuurder] kan geen voorzitter zijn van de ondernemingsraad van de [onderneming].</t>
+  </si>
+  <si>
+    <t>De [bestuurder] is niet verkiesbaar tot lid van de ondernemingsraad van de [onderneming].</t>
+  </si>
+  <si>
+    <t>Binding</t>
+  </si>
+  <si>
+    <t>[Binding]</t>
+  </si>
+  <si>
+    <t>Template</t>
+  </si>
+  <si>
+    <t>[Template]</t>
+  </si>
+  <si>
+    <t>TTextID</t>
   </si>
 </sst>
 </file>
@@ -507,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -526,153 +532,193 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>3</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="7" t="s">
-        <v>34</v>
-      </c>
       <c r="F4" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" s="3" t="s">
+      <c r="B7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="D12" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" s="8" t="s">
+    </row>
+    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>33</v>
+      <c r="F13" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Interfaces and spreadsheet made demonstrable for the binding mechamism.
</commit_message>
<xml_diff>
--- a/MirrorMe/MirrorMe - Example.xlsx
+++ b/MirrorMe/MirrorMe - Example.xlsx
@@ -58,9 +58,6 @@
     <t>Scope</t>
   </si>
   <si>
-    <t>Zaak_X123</t>
-  </si>
-  <si>
     <t>art. 1 lid 1 sub c WOR</t>
   </si>
   <si>
@@ -133,7 +130,10 @@
     <t>[Template]</t>
   </si>
   <si>
-    <t>TTextID</t>
+    <t>Case_X123</t>
+  </si>
+  <si>
+    <t>TTName</t>
   </si>
 </sst>
 </file>
@@ -516,7 +516,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -532,7 +532,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -547,12 +547,12 @@
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>13</v>
@@ -567,7 +567,7 @@
         <v>4</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -575,13 +575,13 @@
         <v>8</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -589,14 +589,14 @@
         <v>12</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -604,13 +604,13 @@
         <v>9</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -618,13 +618,13 @@
         <v>10</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -632,18 +632,18 @@
         <v>11</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>0</v>
@@ -658,12 +658,12 @@
         <v>2</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>13</v>
@@ -678,7 +678,7 @@
         <v>4</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -686,19 +686,19 @@
         <v>6</v>
       </c>
       <c r="B12" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -706,19 +706,19 @@
         <v>7</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="C13" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="4" t="s">
-        <v>23</v>
-      </c>
       <c r="E13" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
working towards an case-based application and Login added.
</commit_message>
<xml_diff>
--- a/MirrorMe/MirrorMe - Example.xlsx
+++ b/MirrorMe/MirrorMe - Example.xlsx
@@ -8,13 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="MirroMe Voorbeeldredenering" sheetId="1" r:id="rId1"/>
+    <sheet name="MirrorMe Example Argument" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="65">
   <si>
     <t>ttScope</t>
   </si>
@@ -134,6 +135,81 @@
   </si>
   <si>
     <t>TTName</t>
+  </si>
+  <si>
+    <t>Case</t>
+  </si>
+  <si>
+    <t>[Case]</t>
+  </si>
+  <si>
+    <t>In applying the WOR or any regulation based on the WOR, the [executive officer] is considered not to be part of the workforce of the [enterprise].</t>
+  </si>
+  <si>
+    <t>Eligible as member of the Enterprise Council are persons who have been employed by the [enterprise] for at least a year.</t>
+  </si>
+  <si>
+    <t>The [executive officer] is not eligible as member of the Enterprise Council of the [enterprise].</t>
+  </si>
+  <si>
+    <t>The Enterprise Council elects a president from its own members.</t>
+  </si>
+  <si>
+    <t>The [executive officer] cannot be president of the Enterprise Council of the [enterprise].</t>
+  </si>
+  <si>
+    <t>The Tax Authority is an enterprise as meant by the Law on Enterprise Councils (WOR), because it is an independently operating organisational entity, in which labour is performed on the basis of a labour-contract or based on a public administrative appointment.</t>
+  </si>
+  <si>
+    <t>The DG-Bel is executive officer as meant by the Law on Enterprise Councils (WOR), because he exercises in the [enterprise] the highest authority in managing labour.</t>
+  </si>
+  <si>
+    <t>executive officer</t>
+  </si>
+  <si>
+    <t>enterprise</t>
+  </si>
+  <si>
+    <t>Case_X638</t>
+  </si>
+  <si>
+    <t>t03</t>
+  </si>
+  <si>
+    <t>t04</t>
+  </si>
+  <si>
+    <t>t05</t>
+  </si>
+  <si>
+    <t>t03, t04</t>
+  </si>
+  <si>
+    <t>t06</t>
+  </si>
+  <si>
+    <t>t07</t>
+  </si>
+  <si>
+    <t>t05, t06</t>
+  </si>
+  <si>
+    <t>t01</t>
+  </si>
+  <si>
+    <t>t02</t>
+  </si>
+  <si>
+    <t>scopeID</t>
+  </si>
+  <si>
+    <t>ScopeID</t>
+  </si>
+  <si>
+    <t>[Template,]</t>
+  </si>
+  <si>
+    <t>requires</t>
   </si>
 </sst>
 </file>
@@ -513,10 +589,269 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="79.42578125" style="9" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="8.85546875" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="4">
+        <v>3</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="4">
+        <v>4</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="4">
+        <v>5</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="4">
+        <v>6</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="4">
+        <v>7</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="3">
+        <v>123</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -549,6 +884,9 @@
       <c r="F1" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -569,16 +907,22 @@
       <c r="F2" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="G2" s="1" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>38</v>
+        <v>51</v>
+      </c>
+      <c r="C3" s="4">
+        <v>3</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>16</v>
@@ -586,14 +930,17 @@
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>12</v>
+        <v>53</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>38</v>
+        <v>51</v>
+      </c>
+      <c r="C4" s="4">
+        <v>4</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="8" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>17</v>
@@ -601,27 +948,33 @@
     </row>
     <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>9</v>
+        <v>54</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>38</v>
+        <v>51</v>
+      </c>
+      <c r="C5" s="4">
+        <v>5</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>10</v>
+        <v>56</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>38</v>
+        <v>51</v>
+      </c>
+      <c r="C6" s="4">
+        <v>6</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>18</v>
@@ -629,16 +982,19 @@
     </row>
     <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>11</v>
+        <v>57</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>38</v>
+        <v>51</v>
+      </c>
+      <c r="C7" s="4">
+        <v>7</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -683,19 +1039,19 @@
     </row>
     <row r="12" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>6</v>
+        <v>59</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>19</v>
+        <v>50</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>14</v>
@@ -703,26 +1059,52 @@
     </row>
     <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>7</v>
+        <v>60</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>22</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>15</v>
       </c>
     </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="3">
+        <v>638</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="7"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
MirrorMe - made it compilable, added some comments & ideas
</commit_message>
<xml_diff>
--- a/MirrorMe/MirrorMe - Example.xlsx
+++ b/MirrorMe/MirrorMe - Example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7380"/>
+    <workbookView xWindow="240" yWindow="168" windowWidth="14808" windowHeight="7380"/>
   </bookViews>
   <sheets>
     <sheet name="MirroMe Voorbeeldredenering" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="67">
   <si>
     <t>ttScope</t>
   </si>
@@ -74,27 +74,12 @@
     <t>art. 7 WOR</t>
   </si>
   <si>
-    <t>onderneming</t>
-  </si>
-  <si>
     <t>Belastingdienst</t>
   </si>
   <si>
-    <t>bestuurder</t>
-  </si>
-  <si>
     <t>DG-Bel</t>
   </si>
   <si>
-    <t>De Belastingdienst is een onderneming in de zin van de Wet op de ondernemingsraden, omdat het een in de maatschappij als zelfstandige eenheid optredend organisatorisch verband is, waarin krachtens arbeidsovereenkomst of krachtens publiekrechtelijke aanstelling arbeid wordt verricht.</t>
-  </si>
-  <si>
-    <t>Voor de toepassing van het bij of krachtens de WOR bepaalde wordt de [bestuurder] geacht niet te behoren tot de in de [onderneming] werkzame personen.</t>
-  </si>
-  <si>
-    <t>Verkiesbaar tot lid van de ondernemingsraad zijn de personen die gedurende ten minste een jaar in de [onderneming] werkzaam zijn geweest.</t>
-  </si>
-  <si>
     <t>De ondernemingsraad kiest uit zijn midden een voorzitter.</t>
   </si>
   <si>
@@ -104,21 +89,12 @@
     <t>TText_05, TText_06</t>
   </si>
   <si>
-    <t>De DG-Bel is bestuurder in de zin van de Wet op de ondernemingsraden, omdat hij in de [onderneming] de hoogste zeggenschap uitoefent bij de leiding van de arbeid.</t>
-  </si>
-  <si>
     <t>legalGround</t>
   </si>
   <si>
     <t>LegalGround</t>
   </si>
   <si>
-    <t>De [bestuurder] kan geen voorzitter zijn van de ondernemingsraad van de [onderneming].</t>
-  </si>
-  <si>
-    <t>De [bestuurder] is niet verkiesbaar tot lid van de ondernemingsraad van de [onderneming].</t>
-  </si>
-  <si>
     <t>Binding</t>
   </si>
   <si>
@@ -210,6 +186,36 @@
   </si>
   <si>
     <t>requires</t>
+  </si>
+  <si>
+    <t>Voor de toepassing van het bij of krachtens de WOR bepaalde wordt [de bestuurder] geacht niet te behoren tot de in [de onderneming] werkzame personen.</t>
+  </si>
+  <si>
+    <t>Verkiesbaar tot lid van de ondernemingsraad zijn de personen die gedurende ten minste een jaar in [de onderneming] werkzaam zijn geweest.</t>
+  </si>
+  <si>
+    <t>[de bestuurder] is niet verkiesbaar tot lid van de ondernemingsraad van [de onderneming].</t>
+  </si>
+  <si>
+    <t>[de bestuurder] kan geen voorzitter zijn van de ondernemingsraad van [de onderneming].</t>
+  </si>
+  <si>
+    <t>[de onderneming] is een onderneming in de zin van de Wet op de ondernemingsraden, omdat het een in de maatschappij als zelfstandige eenheid optredend organisatorisch verband is, waarin krachtens arbeidsovereenkomst of krachtens publiekrechtelijke aanstelling arbeid wordt verricht.</t>
+  </si>
+  <si>
+    <t>de bestuurder</t>
+  </si>
+  <si>
+    <t>de onderneming</t>
+  </si>
+  <si>
+    <t>Albert Heijn</t>
+  </si>
+  <si>
+    <t>Piet van der Kluns</t>
+  </si>
+  <si>
+    <t>[de bestuurder] is bestuurder in de zin van de Wet op de ondernemingsraden, omdat hij in [de onderneming] de hoogste zeggenschap uitoefent bij de leiding van de arbeid.</t>
   </si>
 </sst>
 </file>
@@ -289,8 +295,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Neutraal" xfId="1" builtinId="28"/>
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -303,9 +309,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Kantoor">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -343,7 +349,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kantoor">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -415,7 +421,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kantoor">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -591,22 +597,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="79.42578125" style="9" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" style="3" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="3"/>
+    <col min="1" max="1" width="10.6640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="79.44140625" style="9" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -621,21 +629,21 @@
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>3</v>
@@ -644,101 +652,101 @@
         <v>4</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C3" s="4">
         <v>3</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C4" s="4">
         <v>4</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="8" t="s">
-        <v>25</v>
+        <v>58</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C5" s="4">
         <v>5</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>33</v>
+        <v>59</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C6" s="4">
         <v>6</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C7" s="4">
         <v>7</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>0</v>
@@ -753,18 +761,18 @@
         <v>2</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>3</v>
@@ -773,68 +781,68 @@
         <v>4</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>19</v>
+        <v>63</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>20</v>
+        <v>64</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>21</v>
+        <v>62</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>22</v>
+        <v>65</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>29</v>
+        <v>66</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B17" s="3">
         <v>123</v>
@@ -854,20 +862,20 @@
       <selection activeCell="G1" sqref="G1:G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="79.42578125" style="9" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" style="3" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="3"/>
+    <col min="1" max="1" width="10.6640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="79.44140625" style="9" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -882,21 +890,21 @@
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>3</v>
@@ -905,24 +913,24 @@
         <v>4</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C3" s="4">
         <v>3</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>16</v>
@@ -930,17 +938,17 @@
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C4" s="4">
         <v>4</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="8" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>17</v>
@@ -948,33 +956,33 @@
     </row>
     <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C5" s="4">
         <v>5</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C6" s="4">
         <v>6</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>18</v>
@@ -982,24 +990,24 @@
     </row>
     <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C7" s="4">
         <v>7</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>0</v>
@@ -1014,18 +1022,18 @@
         <v>2</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>3</v>
@@ -1034,24 +1042,24 @@
         <v>4</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>14</v>
@@ -1059,43 +1067,43 @@
     </row>
     <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B17" s="3">
         <v>638</v>

</xml_diff>

<commit_message>
MirrorMe - modifications made to accommodate for the refactoring changes
</commit_message>
<xml_diff>
--- a/MirrorMe/MirrorMe - Example.xlsx
+++ b/MirrorMe/MirrorMe - Example.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="62">
   <si>
     <t>ttScope</t>
   </si>
@@ -83,12 +83,6 @@
     <t>De ondernemingsraad kiest uit zijn midden een voorzitter.</t>
   </si>
   <si>
-    <t>TText_03, TText_04</t>
-  </si>
-  <si>
-    <t>TText_05, TText_06</t>
-  </si>
-  <si>
     <t>legalGround</t>
   </si>
   <si>
@@ -158,18 +152,12 @@
     <t>t05</t>
   </si>
   <si>
-    <t>t03, t04</t>
-  </si>
-  <si>
     <t>t06</t>
   </si>
   <si>
     <t>t07</t>
   </si>
   <si>
-    <t>t05, t06</t>
-  </si>
-  <si>
     <t>t01</t>
   </si>
   <si>
@@ -180,9 +168,6 @@
   </si>
   <si>
     <t>ScopeID</t>
-  </si>
-  <si>
-    <t>[Template,]</t>
   </si>
   <si>
     <t>requires</t>
@@ -595,10 +580,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -612,9 +597,9 @@
     <col min="7" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -629,21 +614,24 @@
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>3</v>
@@ -652,70 +640,76 @@
         <v>4</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C3" s="4">
         <v>3</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C4" s="4">
         <v>4</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="8" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C5" s="4">
         <v>5</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C6" s="4">
         <v>6</v>
@@ -727,26 +721,29 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C7" s="4">
         <v>7</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>0</v>
@@ -761,18 +758,18 @@
         <v>2</v>
       </c>
       <c r="F10" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>3</v>
@@ -781,68 +778,68 @@
         <v>4</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B17" s="3">
         <v>123</v>
@@ -856,10 +853,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G2"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -873,9 +870,9 @@
     <col min="7" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -890,21 +887,24 @@
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>3</v>
@@ -913,101 +913,110 @@
         <v>4</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C3" s="4">
         <v>3</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C4" s="4">
         <v>4</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C5" s="4">
         <v>5</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C6" s="4">
         <v>6</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C7" s="4">
         <v>7</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>0</v>
@@ -1022,18 +1031,18 @@
         <v>2</v>
       </c>
       <c r="F10" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>3</v>
@@ -1042,68 +1051,68 @@
         <v>4</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>19</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B17" s="3">
         <v>638</v>

</xml_diff>